<commit_message>
template view table dan sidebar-analisis
</commit_message>
<xml_diff>
--- a/data/lusita 2.0/data clean/input modal dialog/io.xlsx
+++ b/data/lusita 2.0/data clean/input modal dialog/io.xlsx
@@ -611,11 +611,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:XFD40"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection sqref="A1:E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>